<commit_message>
After Upgradation of Chrome
After Upgradation of Chrome
</commit_message>
<xml_diff>
--- a/Contacts.xlsx
+++ b/Contacts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695"/>
+    <workbookView windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Recipients" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -38,6 +38,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -47,7 +77,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -62,12 +100,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,40 +114,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -123,22 +131,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,7 +147,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,14 +162,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,25 +191,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,7 +347,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,139 +359,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,25 +386,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -459,17 +450,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -485,15 +485,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -503,130 +503,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -990,7 +990,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="3" s="2" customFormat="1" spans="1:3">
       <c r="A3">
-        <v>3065673726</v>
+        <v>3223</v>
       </c>
       <c r="B3"/>
       <c r="C3" s="1"/>

</xml_diff>